<commit_message>
Updates on solution document, DB creation script, DB ERD, data dictionary excel file and xml structure for insert company function
</commit_message>
<xml_diff>
--- a/TaxesCollection DB Data Dictionary.xlsx
+++ b/TaxesCollection DB Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\TopTal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD93AB1-4FBD-4464-9117-C6BEEE9A1F79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CF81C1-29DA-419D-9245-A5E6E55CC7DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E61D19A7-3D35-49FE-A6AB-AB1174689459}"/>
   </bookViews>
@@ -188,13 +188,7 @@
     <t>Must be unique (company_cuit_number_key)</t>
   </si>
   <si>
-    <t>comencement_date</t>
-  </si>
-  <si>
     <t>Company's operations starting date</t>
-  </si>
-  <si>
-    <t>Must not be after current date time (CHK_Comencement_Date)</t>
   </si>
   <si>
     <t>website</t>
@@ -674,9 +668,6 @@
     <t>company_pkey</t>
   </si>
   <si>
-    <t>CHK_Comencement_Date</t>
-  </si>
-  <si>
     <t>CHK_Created_At</t>
   </si>
   <si>
@@ -779,9 +770,6 @@
     <t>created_at &lt;= CURRENT_TIMESTAMP</t>
   </si>
   <si>
-    <t>comencement_date &lt;= CURRENT_TIMESTAMP</t>
-  </si>
-  <si>
     <t>date_of_birth &lt;= CURRENT_TIMESTAMP</t>
   </si>
   <si>
@@ -822,15 +810,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>email (character varying)
-cuit_number (character varying)
-comencement_date (date)
-website (character varying)
-individuals (integer[])
-phone_numbers (character varying[])
-phone_type_ids (integer[])</t>
   </si>
   <si>
     <t>Creates a company into DB along with its ownership relationships and phone numbers, based on an XLM structure</t>
@@ -886,6 +865,27 @@
   </si>
   <si>
     <t>Returns a table with total tax payed by a taxpayer (individual or company) by a particular year and for all months of that year (that a taxpayer did a payment)</t>
+  </si>
+  <si>
+    <t>commencement_date</t>
+  </si>
+  <si>
+    <t>Must not be after current date time (CHK_Commencement_Date)</t>
+  </si>
+  <si>
+    <t>CHK_Commencement_Date</t>
+  </si>
+  <si>
+    <t>commencement_date &lt;= CURRENT_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>email (character varying)
+cuit_number (character varying)
+commencement_date (date)
+website (character varying)
+individuals (integer[])
+phone_numbers (character varying[])
+phone_type_ids (integer[])</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1369,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>7</v>
@@ -1380,7 +1380,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1388,7 +1388,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1396,63 +1396,63 @@
         <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1472,7 +1472,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="37.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="14" bestFit="1" customWidth="1"/>
@@ -1485,7 +1485,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1665,7 +1665,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>33</v>
@@ -1694,7 +1694,7 @@
         <v>35</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>16</v>
@@ -1723,7 +1723,7 @@
         <v>37</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>16</v>
@@ -1752,7 +1752,7 @@
         <v>38</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>16</v>
@@ -1781,7 +1781,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>40</v>
@@ -1810,7 +1810,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>16</v>
@@ -1926,7 +1926,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>16</v>
@@ -1952,10 +1952,10 @@
         <v>44</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>40</v>
@@ -1970,7 +1970,7 @@
         <v>12</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>51</v>
+        <v>224</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>12</v>
@@ -1981,10 +1981,10 @@
         <v>44</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>16</v>
@@ -2065,13 +2065,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>61</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>10</v>
@@ -2086,7 +2086,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>12</v>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>16</v>
@@ -2115,7 +2115,7 @@
         <v>12</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>12</v>
@@ -2123,13 +2123,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>16</v>
@@ -2152,13 +2152,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>16</v>
@@ -2181,13 +2181,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>33</v>
@@ -2210,7 +2210,7 @@
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>24</v>
@@ -2239,7 +2239,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>29</v>
@@ -2268,13 +2268,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>74</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>76</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>10</v>
@@ -2289,7 +2289,7 @@
         <v>12</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>12</v>
@@ -2297,13 +2297,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>33</v>
@@ -2318,7 +2318,7 @@
         <v>32</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>12</v>
@@ -2326,13 +2326,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>33</v>
@@ -2347,7 +2347,7 @@
         <v>44</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>12</v>
@@ -2355,13 +2355,13 @@
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>26</v>
@@ -2376,7 +2376,7 @@
         <v>12</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I31" s="13" t="s">
         <v>28</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>24</v>
@@ -2413,7 +2413,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>29</v>
@@ -2442,13 +2442,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>86</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>10</v>
@@ -2463,7 +2463,7 @@
         <v>12</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>12</v>
@@ -2471,13 +2471,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>33</v>
@@ -2489,10 +2489,10 @@
         <v>12</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I35" s="17" t="s">
         <v>12</v>
@@ -2500,13 +2500,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>33</v>
@@ -2521,7 +2521,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I36" s="17" t="s">
         <v>12</v>
@@ -2529,28 +2529,28 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="E37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="I37" s="17" t="s">
         <v>12</v>
@@ -2558,13 +2558,13 @@
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>26</v>
@@ -2579,7 +2579,7 @@
         <v>12</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I38" s="17" t="s">
         <v>28</v>
@@ -2587,13 +2587,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>33</v>
@@ -2605,10 +2605,10 @@
         <v>12</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I39" s="17" t="s">
         <v>12</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>24</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>29</v>
@@ -2674,13 +2674,13 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>10</v>
@@ -2695,7 +2695,7 @@
         <v>12</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I42" s="13" t="s">
         <v>12</v>
@@ -2703,13 +2703,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>16</v>
@@ -2724,7 +2724,7 @@
         <v>12</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I43" s="13" t="s">
         <v>12</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>24</v>
@@ -2761,7 +2761,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>29</v>
@@ -2790,13 +2790,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>111</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>10</v>
@@ -2811,7 +2811,7 @@
         <v>12</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I46" s="17" t="s">
         <v>12</v>
@@ -2819,13 +2819,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>16</v>
@@ -2840,7 +2840,7 @@
         <v>12</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I47" s="17" t="s">
         <v>12</v>
@@ -2848,7 +2848,7 @@
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>24</v>
@@ -2877,7 +2877,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B49" s="18" t="s">
         <v>29</v>
@@ -2906,13 +2906,13 @@
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>10</v>
@@ -2927,7 +2927,7 @@
         <v>12</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>12</v>
@@ -2935,13 +2935,13 @@
     </row>
     <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>33</v>
@@ -2956,7 +2956,7 @@
         <v>6</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>12</v>
@@ -2964,13 +2964,13 @@
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>16</v>
@@ -2993,13 +2993,13 @@
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>33</v>
@@ -3011,10 +3011,10 @@
         <v>12</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I53" s="13" t="s">
         <v>12</v>
@@ -3022,7 +3022,7 @@
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>24</v>
@@ -3051,7 +3051,7 @@
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>29</v>
@@ -3080,13 +3080,13 @@
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>10</v>
@@ -3101,7 +3101,7 @@
         <v>12</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>12</v>
@@ -3109,13 +3109,13 @@
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>33</v>
@@ -3127,10 +3127,10 @@
         <v>12</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>12</v>
@@ -3138,13 +3138,13 @@
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>16</v>
@@ -3167,13 +3167,13 @@
     </row>
     <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>33</v>
@@ -3185,10 +3185,10 @@
         <v>12</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I59" s="17" t="s">
         <v>12</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>24</v>
@@ -3225,7 +3225,7 @@
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>29</v>
@@ -3269,7 +3269,7 @@
   <cols>
     <col min="1" max="1" width="43.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" style="4" customWidth="1"/>
     <col min="6" max="6" width="42" style="4" bestFit="1" customWidth="1"/>
@@ -3283,218 +3283,218 @@
         <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>161</v>
+        <v>225</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>223</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -3503,27 +3503,27 @@
         <v>47</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3531,220 +3531,220 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -3753,194 +3753,194 @@
         <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>180</v>
-      </c>
       <c r="F30" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -3949,10 +3949,10 @@
         <v>15</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3960,36 +3960,36 @@
         <v>13</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -3997,19 +3997,19 @@
         <v>20</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4017,104 +4017,104 @@
         <v>17</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4139,114 +4139,114 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updates on data dictionary constraints and on DB scripts sql files
</commit_message>
<xml_diff>
--- a/TaxesCollection DB Data Dictionary.xlsx
+++ b/TaxesCollection DB Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trabajo\TopTal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CF81C1-29DA-419D-9245-A5E6E55CC7DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25735672-9E67-4C08-871E-4DC71BAE0032}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E61D19A7-3D35-49FE-A6AB-AB1174689459}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="227">
   <si>
     <t>Atributes</t>
   </si>
@@ -90,16 +90,10 @@
     <t>Varchar</t>
   </si>
   <si>
-    <t>CHK_Type</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
     <t>Email address of the tax payer</t>
-  </si>
-  <si>
-    <t>CHK_Email</t>
   </si>
   <si>
     <t>Tax payer type</t>
@@ -668,9 +662,6 @@
     <t>company_pkey</t>
   </si>
   <si>
-    <t>CHK_Created_At</t>
-  </si>
-  <si>
     <t>company</t>
   </si>
   <si>
@@ -686,18 +677,12 @@
     <t>individual</t>
   </si>
   <si>
-    <t>CHK_Date_Of_Birth</t>
-  </si>
-  <si>
     <t>individual_taxpayer_id_fkey</t>
   </si>
   <si>
     <t>own_rel</t>
   </si>
   <si>
-    <t>CHK_Start_Date</t>
-  </si>
-  <si>
     <t>Foreign key to company table (taxpayer_id column)</t>
   </si>
   <si>
@@ -719,13 +704,7 @@
     <t>Foreign key to individual table (taxpayer_id column)</t>
   </si>
   <si>
-    <t>CHK_Amount</t>
-  </si>
-  <si>
     <t>Must be positive</t>
-  </si>
-  <si>
-    <t>CHK_Payment_Date</t>
   </si>
   <si>
     <t>Foreign key to Tax_Type table</t>
@@ -871,9 +850,6 @@
   </si>
   <si>
     <t>Must not be after current date time (CHK_Commencement_Date)</t>
-  </si>
-  <si>
-    <t>CHK_Commencement_Date</t>
   </si>
   <si>
     <t>commencement_date &lt;= CURRENT_TIMESTAMP</t>
@@ -886,6 +862,27 @@
 individuals (integer[])
 phone_numbers (character varying[])
 phone_type_ids (integer[])</t>
+  </si>
+  <si>
+    <t>Created At date cannot be after current date</t>
+  </si>
+  <si>
+    <t>Commencement date cannot be after current date</t>
+  </si>
+  <si>
+    <t>Birth date cannot be after current date</t>
+  </si>
+  <si>
+    <t>Amount must be a positive value</t>
+  </si>
+  <si>
+    <t>Payment date cannot be after current date</t>
+  </si>
+  <si>
+    <t>Email must have a valid format</t>
+  </si>
+  <si>
+    <t>Type can only be C for Company or I for Individual</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>7</v>
@@ -1380,79 +1377,79 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1485,7 +1482,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -1509,7 +1506,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1549,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>16</v>
@@ -1564,7 +1561,7 @@
         <v>12</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>12</v>
@@ -1575,10 +1572,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>16</v>
@@ -1593,7 +1590,7 @@
         <v>12</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>12</v>
@@ -1604,28 +1601,28 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1633,10 +1630,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>16</v>
@@ -1654,21 +1651,21 @@
         <v>12</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>11</v>
@@ -1680,7 +1677,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>12</v>
@@ -1688,13 +1685,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>16</v>
@@ -1717,13 +1714,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>16</v>
@@ -1746,13 +1743,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>16</v>
@@ -1775,28 +1772,28 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>12</v>
@@ -1804,13 +1801,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>16</v>
@@ -1833,42 +1830,42 @@
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="18" t="s">
+      <c r="E13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>16</v>
@@ -1886,21 +1883,21 @@
         <v>12</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>11</v>
@@ -1912,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>12</v>
@@ -1920,13 +1917,13 @@
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>16</v>
@@ -1941,7 +1938,7 @@
         <v>12</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I16" s="13" t="s">
         <v>12</v>
@@ -1949,16 +1946,16 @@
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>11</v>
@@ -1970,7 +1967,7 @@
         <v>12</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="I17" s="13" t="s">
         <v>12</v>
@@ -1978,13 +1975,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>16</v>
@@ -2007,42 +2004,42 @@
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="E19" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>16</v>
@@ -2060,18 +2057,18 @@
         <v>12</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>59</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>61</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>10</v>
@@ -2086,7 +2083,7 @@
         <v>12</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I21" s="17" t="s">
         <v>12</v>
@@ -2094,13 +2091,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>16</v>
@@ -2115,7 +2112,7 @@
         <v>12</v>
       </c>
       <c r="H22" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I22" s="17" t="s">
         <v>12</v>
@@ -2123,13 +2120,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>16</v>
@@ -2152,13 +2149,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>16</v>
@@ -2181,16 +2178,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>11</v>
@@ -2210,42 +2207,42 @@
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" s="18" t="s">
+      <c r="E26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>16</v>
@@ -2263,18 +2260,18 @@
         <v>12</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>72</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>10</v>
@@ -2289,7 +2286,7 @@
         <v>12</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I28" s="13" t="s">
         <v>12</v>
@@ -2297,16 +2294,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>11</v>
@@ -2315,10 +2312,10 @@
         <v>12</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>12</v>
@@ -2326,16 +2323,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>11</v>
@@ -2344,10 +2341,10 @@
         <v>12</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>12</v>
@@ -2355,71 +2352,71 @@
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="8" t="s">
+      <c r="I31" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="8" t="s">
+      <c r="E32" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>16</v>
@@ -2437,18 +2434,18 @@
         <v>12</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>86</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>10</v>
@@ -2463,7 +2460,7 @@
         <v>12</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I34" s="17" t="s">
         <v>12</v>
@@ -2471,16 +2468,16 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>11</v>
@@ -2489,10 +2486,10 @@
         <v>12</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I35" s="17" t="s">
         <v>12</v>
@@ -2500,16 +2497,16 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E36" s="19" t="s">
         <v>11</v>
@@ -2521,7 +2518,7 @@
         <v>6</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I36" s="17" t="s">
         <v>12</v>
@@ -2529,28 +2526,28 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="E37" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>95</v>
       </c>
       <c r="I37" s="17" t="s">
         <v>12</v>
@@ -2558,57 +2555,57 @@
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B38" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="18" t="s">
+      <c r="I38" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>100</v>
-      </c>
-      <c r="D39" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>102</v>
       </c>
       <c r="I39" s="17" t="s">
         <v>12</v>
@@ -2616,42 +2613,42 @@
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B40" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D40" s="18" t="s">
+      <c r="E40" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I40" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>16</v>
@@ -2669,18 +2666,18 @@
         <v>12</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>10</v>
@@ -2695,7 +2692,7 @@
         <v>12</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I42" s="13" t="s">
         <v>12</v>
@@ -2703,13 +2700,13 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>16</v>
@@ -2724,7 +2721,7 @@
         <v>12</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I43" s="13" t="s">
         <v>12</v>
@@ -2732,42 +2729,42 @@
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="E44" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I44" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>16</v>
@@ -2785,18 +2782,18 @@
         <v>12</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>107</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>109</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>10</v>
@@ -2811,7 +2808,7 @@
         <v>12</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I46" s="17" t="s">
         <v>12</v>
@@ -2819,13 +2816,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>15</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>16</v>
@@ -2840,7 +2837,7 @@
         <v>12</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I47" s="17" t="s">
         <v>12</v>
@@ -2848,42 +2845,42 @@
     </row>
     <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B48" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" s="18" t="s">
+      <c r="E48" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I48" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F48" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>16</v>
@@ -2901,18 +2898,18 @@
         <v>12</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>10</v>
@@ -2927,7 +2924,7 @@
         <v>12</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>12</v>
@@ -2935,16 +2932,16 @@
     </row>
     <row r="51" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>11</v>
@@ -2956,7 +2953,7 @@
         <v>6</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>12</v>
@@ -2964,13 +2961,13 @@
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>16</v>
@@ -2993,28 +2990,28 @@
     </row>
     <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H53" s="13" t="s">
         <v>125</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>127</v>
       </c>
       <c r="I53" s="13" t="s">
         <v>12</v>
@@ -3022,42 +3019,42 @@
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D54" s="8" t="s">
+      <c r="E54" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I54" s="13" t="s">
         <v>26</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H54" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I54" s="13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>16</v>
@@ -3075,18 +3072,18 @@
         <v>12</v>
       </c>
       <c r="I55" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>10</v>
@@ -3101,7 +3098,7 @@
         <v>12</v>
       </c>
       <c r="H56" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I56" s="17" t="s">
         <v>12</v>
@@ -3109,16 +3106,16 @@
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>11</v>
@@ -3127,10 +3124,10 @@
         <v>12</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H57" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I57" s="17" t="s">
         <v>12</v>
@@ -3138,13 +3135,13 @@
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>16</v>
@@ -3167,28 +3164,28 @@
     </row>
     <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="H59" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F59" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H59" s="17" t="s">
-        <v>131</v>
       </c>
       <c r="I59" s="17" t="s">
         <v>12</v>
@@ -3196,42 +3193,42 @@
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B60" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D60" s="18" t="s">
+      <c r="E60" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G60" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H60" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="I60" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>16</v>
@@ -3249,7 +3246,7 @@
         <v>12</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3267,7 +3264,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -3283,468 +3280,468 @@
         <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>165</v>
+        <v>222</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
@@ -3753,194 +3750,194 @@
         <v>15</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>176</v>
+        <v>223</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
@@ -3949,10 +3946,10 @@
         <v>15</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -3960,161 +3957,161 @@
         <v>13</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>20</v>
+        <v>225</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>17</v>
+        <v>226</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4139,114 +4136,114 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>